<commit_message>
creating final version & pred file
</commit_message>
<xml_diff>
--- a/Predictions_file.xlsx
+++ b/Predictions_file.xlsx
@@ -597,7 +597,7 @@
         <v>-3.8</v>
       </c>
       <c r="Z2">
-        <v>8.530396666666668</v>
+        <v>8.542825333333337</v>
       </c>
       <c r="AA2">
         <v>0.022</v>
@@ -700,7 +700,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z3">
-        <v>8.43421800000001</v>
+        <v>8.431724000000004</v>
       </c>
       <c r="AA3">
         <v>0.03</v>
@@ -803,7 +803,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z4">
-        <v>8.494688666666676</v>
+        <v>8.506146666666675</v>
       </c>
       <c r="AA4">
         <v>0.046</v>
@@ -900,7 +900,7 @@
         <v>-4</v>
       </c>
       <c r="Z5">
-        <v>8.531116666666671</v>
+        <v>8.519511333333336</v>
       </c>
       <c r="AB5">
         <v>120</v>
@@ -1000,7 +1000,7 @@
         <v>-4</v>
       </c>
       <c r="Z6">
-        <v>8.471594000000009</v>
+        <v>8.48036066666668</v>
       </c>
       <c r="AA6">
         <v>0.082</v>
@@ -1100,7 +1100,7 @@
         <v>-3.8</v>
       </c>
       <c r="Z7">
-        <v>8.532068000000001</v>
+        <v>8.512123333333324</v>
       </c>
       <c r="AA7">
         <v>0.064</v>
@@ -1203,7 +1203,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z8">
-        <v>8.497293333333342</v>
+        <v>8.49545066666666</v>
       </c>
       <c r="AA8">
         <v>0.042</v>
@@ -1297,7 +1297,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z9">
-        <v>8.54385933333333</v>
+        <v>8.545331999999991</v>
       </c>
       <c r="AA9">
         <v>0.096</v>
@@ -1400,7 +1400,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z10">
-        <v>8.55661866666666</v>
+        <v>8.551910666666661</v>
       </c>
       <c r="AA10">
         <v>0.046</v>
@@ -1500,7 +1500,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z11">
-        <v>8.594369333333331</v>
+        <v>8.588697999999994</v>
       </c>
       <c r="AA11">
         <v>0.096</v>
@@ -1597,7 +1597,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z12">
-        <v>8.54142133333333</v>
+        <v>8.550192666666657</v>
       </c>
       <c r="AA12">
         <v>0.066</v>
@@ -1700,7 +1700,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z13">
-        <v>8.525820666666668</v>
+        <v>8.533559333333326</v>
       </c>
       <c r="AA13">
         <v>0.048</v>
@@ -1803,7 +1803,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z14">
-        <v>8.448748666666676</v>
+        <v>8.451910000000003</v>
       </c>
       <c r="AA14">
         <v>0.066</v>
@@ -1906,7 +1906,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z15">
-        <v>8.647936666666665</v>
+        <v>8.64379933333333</v>
       </c>
       <c r="AA15">
         <v>0.05</v>
@@ -2009,7 +2009,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z16">
-        <v>8.230284666666648</v>
+        <v>8.230000666666641</v>
       </c>
       <c r="AA16">
         <v>0.046</v>
@@ -2101,7 +2101,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z17">
-        <v>8.634828666666662</v>
+        <v>8.640202666666667</v>
       </c>
       <c r="AA17">
         <v>0.16</v>
@@ -2204,7 +2204,7 @@
         <v>-4</v>
       </c>
       <c r="Z18">
-        <v>8.593359999999992</v>
+        <v>8.583688000000002</v>
       </c>
       <c r="AA18">
         <v>0.102</v>
@@ -2307,7 +2307,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z19">
-        <v>8.527410666666679</v>
+        <v>8.511490000000009</v>
       </c>
       <c r="AA19">
         <v>0.06</v>
@@ -2410,7 +2410,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z20">
-        <v>8.512719333333335</v>
+        <v>8.512406666666656</v>
       </c>
       <c r="AA20">
         <v>0.154</v>
@@ -2513,7 +2513,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z21">
-        <v>8.684074000000008</v>
+        <v>8.678246666666674</v>
       </c>
       <c r="AA21">
         <v>0.022</v>
@@ -2616,7 +2616,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z22">
-        <v>8.685844000000014</v>
+        <v>8.681921333333335</v>
       </c>
       <c r="AA22">
         <v>0.022</v>
@@ -2716,7 +2716,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z23">
-        <v>8.646776666666666</v>
+        <v>8.658210666666664</v>
       </c>
       <c r="AA23">
         <v>0.054</v>
@@ -2813,7 +2813,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z24">
-        <v>8.605871999999987</v>
+        <v>8.619527333333325</v>
       </c>
       <c r="AA24">
         <v>0.022</v>
@@ -2916,7 +2916,7 @@
         <v>-4</v>
       </c>
       <c r="Z25">
-        <v>8.598488666666659</v>
+        <v>8.600998666666658</v>
       </c>
       <c r="AA25">
         <v>0.022</v>
@@ -3019,7 +3019,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z26">
-        <v>8.654605333333343</v>
+        <v>8.647554000000005</v>
       </c>
       <c r="AA26">
         <v>0.024</v>
@@ -3122,7 +3122,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z27">
-        <v>8.48418266666665</v>
+        <v>8.492537333333322</v>
       </c>
       <c r="AA27">
         <v>0.022</v>
@@ -3225,7 +3225,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z28">
-        <v>8.325467999999979</v>
+        <v>8.330583333333317</v>
       </c>
       <c r="AA28">
         <v>0.022</v>
@@ -3328,7 +3328,7 @@
         <v>-3.8</v>
       </c>
       <c r="Z29">
-        <v>8.657124666666634</v>
+        <v>8.659925999999986</v>
       </c>
       <c r="AA29">
         <v>0.174</v>
@@ -3428,7 +3428,7 @@
         <v>-3.8</v>
       </c>
       <c r="Z30">
-        <v>8.662187333333323</v>
+        <v>8.654437999999978</v>
       </c>
       <c r="AA30">
         <v>0.022</v>
@@ -3531,7 +3531,7 @@
         <v>-4</v>
       </c>
       <c r="Z31">
-        <v>8.664984666666642</v>
+        <v>8.657923333333299</v>
       </c>
       <c r="AA31">
         <v>0.024</v>
@@ -3634,7 +3634,7 @@
         <v>-4</v>
       </c>
       <c r="Z32">
-        <v>8.621423999999983</v>
+        <v>8.633210666666656</v>
       </c>
       <c r="AA32">
         <v>0.066</v>
@@ -3734,7 +3734,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z33">
-        <v>8.70987</v>
+        <v>8.709503999999999</v>
       </c>
       <c r="AA33">
         <v>0.024</v>
@@ -3834,7 +3834,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z34">
-        <v>8.646182666666659</v>
+        <v>8.648805999999983</v>
       </c>
       <c r="AA34">
         <v>0.022</v>
@@ -3934,7 +3934,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z35">
-        <v>8.662612666666648</v>
+        <v>8.654977333333315</v>
       </c>
       <c r="AA35">
         <v>0.022</v>
@@ -4034,7 +4034,7 @@
         <v>-4</v>
       </c>
       <c r="Z36">
-        <v>8.685715999999999</v>
+        <v>8.687091333333319</v>
       </c>
       <c r="AA36">
         <v>0.036</v>
@@ -4137,7 +4137,7 @@
         <v>-4</v>
       </c>
       <c r="Z37">
-        <v>8.60842999999999</v>
+        <v>8.613979999999982</v>
       </c>
       <c r="AA37">
         <v>0.022</v>
@@ -4240,7 +4240,7 @@
         <v>-3.6</v>
       </c>
       <c r="Z38">
-        <v>8.558829333333327</v>
+        <v>8.566584666666653</v>
       </c>
       <c r="AA38">
         <v>0.022</v>
@@ -4343,7 +4343,7 @@
         <v>-3.6</v>
       </c>
       <c r="Z39">
-        <v>8.552809333333323</v>
+        <v>8.560773999999977</v>
       </c>
       <c r="AA39">
         <v>0.022</v>
@@ -4446,7 +4446,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z40">
-        <v>8.656335999999985</v>
+        <v>8.667040666666653</v>
       </c>
       <c r="AA40">
         <v>0.052</v>
@@ -4546,7 +4546,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z41">
-        <v>8.736074666666665</v>
+        <v>8.732675999999994</v>
       </c>
       <c r="AA41">
         <v>0.05</v>
@@ -4649,7 +4649,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z42">
-        <v>8.76496600000001</v>
+        <v>8.760124000000015</v>
       </c>
       <c r="AA42">
         <v>0.042</v>
@@ -4749,7 +4749,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z43">
-        <v>8.617389333333357</v>
+        <v>8.633572000000019</v>
       </c>
       <c r="AA43">
         <v>0.024</v>
@@ -4852,7 +4852,7 @@
         <v>-5</v>
       </c>
       <c r="Z44">
-        <v>8.260842666666647</v>
+        <v>8.247153999999973</v>
       </c>
       <c r="AA44">
         <v>0.022</v>
@@ -4955,7 +4955,7 @@
         <v>-5</v>
       </c>
       <c r="Z45">
-        <v>8.226523333333308</v>
+        <v>8.218973333333302</v>
       </c>
       <c r="AA45">
         <v>0.022</v>
@@ -5058,7 +5058,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z46">
-        <v>8.716386666666661</v>
+        <v>8.729265333333334</v>
       </c>
       <c r="AA46">
         <v>0.024</v>
@@ -5161,7 +5161,7 @@
         <v>-5</v>
       </c>
       <c r="Z47">
-        <v>8.762432000000018</v>
+        <v>8.752030000000014</v>
       </c>
       <c r="AA47">
         <v>0.036</v>
@@ -5264,7 +5264,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z48">
-        <v>8.739886</v>
+        <v>8.729178000000005</v>
       </c>
       <c r="AA48">
         <v>0.036</v>
@@ -5367,7 +5367,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z49">
-        <v>8.705344666666662</v>
+        <v>8.695565333333327</v>
       </c>
       <c r="AA49">
         <v>0.024</v>
@@ -5470,7 +5470,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z50">
-        <v>8.694189999999999</v>
+        <v>8.695070666666654</v>
       </c>
       <c r="AA50">
         <v>0.024</v>
@@ -5573,7 +5573,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z51">
-        <v>8.782709333333349</v>
+        <v>8.778133333333351</v>
       </c>
       <c r="AA51">
         <v>0.024</v>
@@ -5670,7 +5670,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z52">
-        <v>8.66220466666665</v>
+        <v>8.66509666666666</v>
       </c>
       <c r="AA52">
         <v>0.07000000000000001</v>
@@ -5773,7 +5773,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z53">
-        <v>8.712042666666665</v>
+        <v>8.721697333333331</v>
       </c>
       <c r="AA53">
         <v>0.022</v>
@@ -5873,7 +5873,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z54">
-        <v>8.698210666666663</v>
+        <v>8.699183333333332</v>
       </c>
       <c r="AA54">
         <v>0.122</v>
@@ -5973,7 +5973,7 @@
         <v>-5</v>
       </c>
       <c r="Z55">
-        <v>8.751753333333333</v>
+        <v>8.755021333333353</v>
       </c>
       <c r="AA55">
         <v>0.024</v>
@@ -6076,7 +6076,7 @@
         <v>-5</v>
       </c>
       <c r="Z56">
-        <v>8.770068000000014</v>
+        <v>8.772191333333351</v>
       </c>
       <c r="AA56">
         <v>0.024</v>
@@ -6179,7 +6179,7 @@
         <v>-5</v>
       </c>
       <c r="Z57">
-        <v>8.742214666666682</v>
+        <v>8.733416666666672</v>
       </c>
       <c r="AA57">
         <v>0.042</v>
@@ -6282,7 +6282,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z58">
-        <v>8.47922999999999</v>
+        <v>8.478177333333331</v>
       </c>
       <c r="AA58">
         <v>0.12</v>
@@ -6385,7 +6385,7 @@
         <v>-5</v>
       </c>
       <c r="Z59">
-        <v>8.506765999999985</v>
+        <v>8.496440666666647</v>
       </c>
       <c r="AA59">
         <v>0.068</v>
@@ -6488,7 +6488,7 @@
         <v>-5</v>
       </c>
       <c r="Z60">
-        <v>8.711223999999973</v>
+        <v>8.714651999999987</v>
       </c>
       <c r="AA60">
         <v>0.066</v>
@@ -6591,7 +6591,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z61">
-        <v>8.769124666666675</v>
+        <v>8.773218000000009</v>
       </c>
       <c r="AA61">
         <v>0.042</v>
@@ -6694,7 +6694,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z62">
-        <v>8.765052000000018</v>
+        <v>8.761890666666678</v>
       </c>
       <c r="AA62">
         <v>0.058</v>
@@ -6797,7 +6797,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z63">
-        <v>8.737734000000012</v>
+        <v>8.751200666666691</v>
       </c>
       <c r="AA63">
         <v>0.058</v>
@@ -6900,7 +6900,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z64">
-        <v>8.779568000000022</v>
+        <v>8.786116666666699</v>
       </c>
       <c r="AA64">
         <v>0.092</v>
@@ -7003,7 +7003,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z65">
-        <v>8.770052000000014</v>
+        <v>8.790490000000016</v>
       </c>
       <c r="AA65">
         <v>0.146</v>
@@ -7106,7 +7106,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z66">
-        <v>8.791012666666685</v>
+        <v>8.804093333333364</v>
       </c>
       <c r="AA66">
         <v>0.108</v>
@@ -7209,7 +7209,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z67">
-        <v>8.760242666666674</v>
+        <v>8.771529333333349</v>
       </c>
       <c r="AA67">
         <v>0.05</v>
@@ -7312,7 +7312,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z68">
-        <v>8.586277999999988</v>
+        <v>8.575722666666652</v>
       </c>
       <c r="AA68">
         <v>0.158</v>
@@ -7415,7 +7415,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z69">
-        <v>8.60270466666665</v>
+        <v>8.597685333333324</v>
       </c>
       <c r="AA69">
         <v>0.138</v>
@@ -7518,7 +7518,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z70">
-        <v>8.588453333333314</v>
+        <v>8.591078666666645</v>
       </c>
       <c r="AA70">
         <v>0.132</v>
@@ -7621,7 +7621,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z71">
-        <v>8.559392666666657</v>
+        <v>8.564785333333321</v>
       </c>
       <c r="AA71">
         <v>0.172</v>
@@ -7724,7 +7724,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z72">
-        <v>8.498397333333337</v>
+        <v>8.492103333333322</v>
       </c>
       <c r="AA72">
         <v>0.22</v>
@@ -7827,7 +7827,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z73">
-        <v>8.330127333333367</v>
+        <v>8.331549333333362</v>
       </c>
       <c r="AA73">
         <v>0.126</v>
@@ -7930,7 +7930,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z74">
-        <v>8.540150666666664</v>
+        <v>8.532263999999994</v>
       </c>
       <c r="AA74">
         <v>0.08599999999999999</v>
@@ -8033,7 +8033,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z75">
-        <v>8.539710666666659</v>
+        <v>8.541210666666659</v>
       </c>
       <c r="AA75">
         <v>0.116</v>
@@ -8136,7 +8136,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z76">
-        <v>8.53388066666667</v>
+        <v>8.533363333333329</v>
       </c>
       <c r="AA76">
         <v>0.068</v>
@@ -8239,7 +8239,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z77">
-        <v>8.524457333333329</v>
+        <v>8.52079</v>
       </c>
       <c r="AA77">
         <v>0.06</v>
@@ -8342,7 +8342,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z78">
-        <v>8.586531333333319</v>
+        <v>8.583505999999986</v>
       </c>
       <c r="AA78">
         <v>0.044</v>
@@ -8442,7 +8442,7 @@
         <v>-5</v>
       </c>
       <c r="Z79">
-        <v>8.669787333333344</v>
+        <v>8.686403999999984</v>
       </c>
       <c r="AA79">
         <v>0.076</v>
@@ -8545,7 +8545,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z80">
-        <v>8.706733999999976</v>
+        <v>8.715625333333328</v>
       </c>
       <c r="AA80">
         <v>0.058</v>
@@ -8648,7 +8648,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z81">
-        <v>8.68923866666665</v>
+        <v>8.687581999999979</v>
       </c>
       <c r="AA81">
         <v>0.052</v>
@@ -8751,7 +8751,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z82">
-        <v>8.779223333333357</v>
+        <v>8.783737333333359</v>
       </c>
       <c r="AA82">
         <v>0.07000000000000001</v>
@@ -8854,7 +8854,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z83">
-        <v>8.667404666666657</v>
+        <v>8.672131999999998</v>
       </c>
       <c r="AA83">
         <v>0.168</v>
@@ -8957,7 +8957,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z84">
-        <v>8.665634666666664</v>
+        <v>8.678568666666665</v>
       </c>
       <c r="AA84">
         <v>0.17</v>
@@ -9060,7 +9060,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z85">
-        <v>8.64894466666667</v>
+        <v>8.643412000000005</v>
       </c>
       <c r="AA85">
         <v>0.09</v>
@@ -9154,7 +9154,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z86">
-        <v>8.715147333333338</v>
+        <v>8.723284000000005</v>
       </c>
       <c r="AB86">
         <v>120</v>
@@ -9251,7 +9251,7 @@
         <v>-5</v>
       </c>
       <c r="Z87">
-        <v>8.708061999999993</v>
+        <v>8.716014666666673</v>
       </c>
       <c r="AA87">
         <v>0.068</v>
@@ -9354,7 +9354,7 @@
         <v>-5</v>
       </c>
       <c r="Z88">
-        <v>8.737780666666648</v>
+        <v>8.744100666666649</v>
       </c>
       <c r="AA88">
         <v>0.046</v>
@@ -9457,7 +9457,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z89">
-        <v>8.67529999999997</v>
+        <v>8.682223999999959</v>
       </c>
       <c r="AA89">
         <v>0.066</v>
@@ -9560,7 +9560,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z90">
-        <v>8.562598000000001</v>
+        <v>8.545444666666652</v>
       </c>
       <c r="AA90">
         <v>0.194</v>
@@ -9663,7 +9663,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z91">
-        <v>8.722358666666667</v>
+        <v>8.730513333333327</v>
       </c>
       <c r="AA91">
         <v>0.082</v>
@@ -9763,7 +9763,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z92">
-        <v>8.680725999999989</v>
+        <v>8.676011999999991</v>
       </c>
       <c r="AA92">
         <v>0.08400000000000001</v>
@@ -9839,7 +9839,7 @@
         <v>3.48</v>
       </c>
       <c r="Z93">
-        <v>8.667897333333336</v>
+        <v>8.650542000000002</v>
       </c>
       <c r="AC93">
         <v>46</v>
@@ -9927,7 +9927,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z94">
-        <v>8.540594666666664</v>
+        <v>8.534259999999984</v>
       </c>
       <c r="AA94">
         <v>0.354</v>
@@ -10027,7 +10027,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z95">
-        <v>8.537042666666665</v>
+        <v>8.543578666666654</v>
       </c>
       <c r="AA95">
         <v>0.398</v>
@@ -10127,7 +10127,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z96">
-        <v>8.602934666666654</v>
+        <v>8.597649333333328</v>
       </c>
       <c r="AA96">
         <v>0.186</v>
@@ -10230,7 +10230,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z97">
-        <v>8.638767333333311</v>
+        <v>8.643512666666656</v>
       </c>
       <c r="AA97">
         <v>0.07199999999999999</v>
@@ -10327,7 +10327,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z98">
-        <v>8.629513999999977</v>
+        <v>8.620725333333306</v>
       </c>
       <c r="AA98">
         <v>0.04</v>
@@ -10430,7 +10430,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z99">
-        <v>8.678103999999983</v>
+        <v>8.670711333333314</v>
       </c>
       <c r="AA99">
         <v>0.07000000000000001</v>
@@ -10530,7 +10530,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z100">
-        <v>8.673826666666653</v>
+        <v>8.673311333333311</v>
       </c>
       <c r="AA100">
         <v>0.058</v>
@@ -10633,7 +10633,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z101">
-        <v>8.675077999999989</v>
+        <v>8.678931333333315</v>
       </c>
       <c r="AA101">
         <v>0.066</v>
@@ -10733,7 +10733,7 @@
         <v>-5</v>
       </c>
       <c r="Z102">
-        <v>8.662350666666663</v>
+        <v>8.670403999999996</v>
       </c>
       <c r="AA102">
         <v>0.058</v>
@@ -10836,7 +10836,7 @@
         <v>-5</v>
       </c>
       <c r="Z103">
-        <v>8.694217333333329</v>
+        <v>8.706496666666657</v>
       </c>
       <c r="AA103">
         <v>0.104</v>
@@ -10939,7 +10939,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z104">
-        <v>8.691101999999972</v>
+        <v>8.694777333333304</v>
       </c>
       <c r="AA104">
         <v>0.108</v>
@@ -11042,7 +11042,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z105">
-        <v>8.70049066666666</v>
+        <v>8.701702666666666</v>
       </c>
       <c r="AA105">
         <v>0.116</v>
@@ -11145,7 +11145,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z106">
-        <v>8.780698000000008</v>
+        <v>8.780743333333339</v>
       </c>
       <c r="AA106">
         <v>0.08</v>
@@ -11248,7 +11248,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z107">
-        <v>8.772480000000009</v>
+        <v>8.771524000000015</v>
       </c>
       <c r="AA107">
         <v>0.052</v>
@@ -11351,7 +11351,7 @@
         <v>-5</v>
       </c>
       <c r="Z108">
-        <v>8.492890666666662</v>
+        <v>8.488102666666661</v>
       </c>
       <c r="AA108">
         <v>0.184</v>
@@ -11454,7 +11454,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z109">
-        <v>8.435809999999998</v>
+        <v>8.421114666666664</v>
       </c>
       <c r="AA109">
         <v>0.122</v>
@@ -11557,7 +11557,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z110">
-        <v>8.507765333333335</v>
+        <v>8.506121999999994</v>
       </c>
       <c r="AA110">
         <v>0.116</v>
@@ -11657,7 +11657,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z111">
-        <v>8.476973333333328</v>
+        <v>8.482867333333322</v>
       </c>
       <c r="AA111">
         <v>0.08799999999999999</v>
@@ -11760,7 +11760,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z112">
-        <v>8.681857333333308</v>
+        <v>8.690607333333292</v>
       </c>
       <c r="AA112">
         <v>0.074</v>
@@ -11863,7 +11863,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z113">
-        <v>8.692630666666629</v>
+        <v>8.693122666666628</v>
       </c>
       <c r="AA113">
         <v>0.07199999999999999</v>
@@ -11966,7 +11966,7 @@
         <v>-5</v>
       </c>
       <c r="Z114">
-        <v>8.676573999999988</v>
+        <v>8.692291333333335</v>
       </c>
       <c r="AA114">
         <v>0.06</v>
@@ -12069,7 +12069,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z115">
-        <v>8.712051333333333</v>
+        <v>8.719895333333326</v>
       </c>
       <c r="AA115">
         <v>0.054</v>
@@ -12166,7 +12166,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z116">
-        <v>8.650081333333317</v>
+        <v>8.63913999999998</v>
       </c>
       <c r="AA116">
         <v>0.116</v>
@@ -12269,7 +12269,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z117">
-        <v>8.71921466666665</v>
+        <v>8.719067333333308</v>
       </c>
       <c r="AA117">
         <v>0.0056</v>
@@ -12372,7 +12372,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z118">
-        <v>8.729202666666632</v>
+        <v>8.729241333333311</v>
       </c>
       <c r="AA118">
         <v>0.008800000000000001</v>
@@ -12472,7 +12472,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z119">
-        <v>8.714027333333338</v>
+        <v>8.711969333333327</v>
       </c>
       <c r="AA119">
         <v>0.0052</v>
@@ -12575,7 +12575,7 @@
         <v>-5</v>
       </c>
       <c r="Z120">
-        <v>8.723169999999989</v>
+        <v>8.728826666666661</v>
       </c>
       <c r="AA120">
         <v>0.0076</v>
@@ -12678,7 +12678,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z121">
-        <v>8.691229999999987</v>
+        <v>8.695353333333317</v>
       </c>
       <c r="AA121">
         <v>0.0114</v>
@@ -12778,7 +12778,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z122">
-        <v>8.679594666666645</v>
+        <v>8.693523333333305</v>
       </c>
       <c r="AA122">
         <v>0.008800000000000001</v>
@@ -12881,7 +12881,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z123">
-        <v>8.712775333333333</v>
+        <v>8.720727999999994</v>
       </c>
       <c r="AA123">
         <v>0.007</v>
@@ -12984,7 +12984,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z124">
-        <v>8.730036666666644</v>
+        <v>8.736038666666659</v>
       </c>
       <c r="AA124">
         <v>0.007</v>
@@ -13087,7 +13087,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z125">
-        <v>8.686364000000014</v>
+        <v>8.674370000000014</v>
       </c>
       <c r="AA125">
         <v>0.008399999999999999</v>
@@ -13190,7 +13190,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z126">
-        <v>8.538663999999997</v>
+        <v>8.543777999999993</v>
       </c>
       <c r="AA126">
         <v>0.0066</v>
@@ -13293,7 +13293,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z127">
-        <v>8.413637999999995</v>
+        <v>8.398950000000003</v>
       </c>
       <c r="AA127">
         <v>0.005</v>
@@ -13391,7 +13391,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z128">
-        <v>8.512041333333332</v>
+        <v>8.506114666666672</v>
       </c>
       <c r="AA128">
         <v>0.0094</v>
@@ -13494,7 +13494,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z129">
-        <v>8.303167333333358</v>
+        <v>8.308206666666697</v>
       </c>
       <c r="AA129">
         <v>0.0184</v>
@@ -13594,7 +13594,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z130">
-        <v>8.458453333333342</v>
+        <v>8.464766666666678</v>
       </c>
       <c r="AA130">
         <v>0.008</v>
@@ -13697,7 +13697,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z131">
-        <v>8.482367333333338</v>
+        <v>8.478044666666674</v>
       </c>
       <c r="AA131">
         <v>0.008800000000000001</v>
@@ -13797,7 +13797,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z132">
-        <v>8.538843999999989</v>
+        <v>8.537375999999997</v>
       </c>
       <c r="AA132">
         <v>0.0072</v>
@@ -13897,7 +13897,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z133">
-        <v>8.537270666666666</v>
+        <v>8.53559866666666</v>
       </c>
       <c r="AA133">
         <v>0.0098</v>
@@ -13997,7 +13997,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z134">
-        <v>8.478116666666661</v>
+        <v>8.511165333333334</v>
       </c>
       <c r="AA134">
         <v>0.0264</v>
@@ -14094,7 +14094,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z135">
-        <v>8.473713333333336</v>
+        <v>8.478648666666674</v>
       </c>
       <c r="AA135">
         <v>0.0108</v>
@@ -14197,7 +14197,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z136">
-        <v>8.480512666666669</v>
+        <v>8.474825333333341</v>
       </c>
       <c r="AA136">
         <v>0.0114</v>
@@ -14300,7 +14300,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z137">
-        <v>8.51754399999998</v>
+        <v>8.515953333333318</v>
       </c>
       <c r="AA137">
         <v>0.0194</v>
@@ -14397,7 +14397,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z138">
-        <v>8.454052000000006</v>
+        <v>8.462911333333349</v>
       </c>
       <c r="AA138">
         <v>0.0466</v>
@@ -14497,7 +14497,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z139">
-        <v>8.548058000000008</v>
+        <v>8.592634666666667</v>
       </c>
       <c r="AA139">
         <v>0.0434</v>
@@ -14597,7 +14597,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z140">
-        <v>8.411922666666705</v>
+        <v>8.415058000000034</v>
       </c>
       <c r="AA140">
         <v>0.0436</v>
@@ -14697,7 +14697,7 @@
         <v>-5</v>
       </c>
       <c r="Z141">
-        <v>8.416209333333367</v>
+        <v>8.420824666666704</v>
       </c>
       <c r="AA141">
         <v>0.0468</v>
@@ -14800,7 +14800,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z142">
-        <v>8.461062666666681</v>
+        <v>8.455588666666683</v>
       </c>
       <c r="AA142">
         <v>0.0454</v>
@@ -14903,7 +14903,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z143">
-        <v>8.501472000000005</v>
+        <v>8.498255333333331</v>
       </c>
       <c r="AA143">
         <v>0.052</v>
@@ -15006,7 +15006,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z144">
-        <v>8.47235666666667</v>
+        <v>8.463845333333341</v>
       </c>
       <c r="AA144">
         <v>0.0572</v>
@@ -15109,7 +15109,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z145">
-        <v>8.524737999999996</v>
+        <v>8.535971333333324</v>
       </c>
       <c r="AA145">
         <v>0.0374</v>
@@ -15209,7 +15209,7 @@
         <v>-6.2</v>
       </c>
       <c r="Z146">
-        <v>8.420724000000007</v>
+        <v>8.414924000000006</v>
       </c>
       <c r="AA146">
         <v>0.0322</v>
@@ -15312,7 +15312,7 @@
         <v>-6.2</v>
       </c>
       <c r="Z147">
-        <v>8.500333333333327</v>
+        <v>8.498381999999998</v>
       </c>
       <c r="AA147">
         <v>0.033</v>
@@ -15415,7 +15415,7 @@
         <v>-6.2</v>
       </c>
       <c r="Z148">
-        <v>8.491364666666668</v>
+        <v>8.48956533333333</v>
       </c>
       <c r="AA148">
         <v>0.0332</v>
@@ -15518,7 +15518,7 @@
         <v>-6.2</v>
       </c>
       <c r="Z149">
-        <v>8.540099999999981</v>
+        <v>8.539038666666652</v>
       </c>
       <c r="AA149">
         <v>0.0364</v>
@@ -15618,7 +15618,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z150">
-        <v>8.467663333333341</v>
+        <v>8.476468000000001</v>
       </c>
       <c r="AA150">
         <v>0.0444</v>
@@ -15721,7 +15721,7 @@
         <v>-6</v>
       </c>
       <c r="Z151">
-        <v>8.580765999999976</v>
+        <v>8.578077333333304</v>
       </c>
       <c r="AA151">
         <v>0.0414</v>
@@ -15824,7 +15824,7 @@
         <v>-6</v>
       </c>
       <c r="Z152">
-        <v>8.606107333333313</v>
+        <v>8.605983333333304</v>
       </c>
       <c r="AA152">
         <v>0.0414</v>
@@ -15927,7 +15927,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z153">
-        <v>8.556461999999977</v>
+        <v>8.561715333333312</v>
       </c>
       <c r="AA153">
         <v>0.0372</v>
@@ -16030,7 +16030,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z154">
-        <v>8.483320000000004</v>
+        <v>8.492359999999998</v>
       </c>
       <c r="AA154">
         <v>0.034</v>
@@ -16133,7 +16133,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z155">
-        <v>8.663397999999974</v>
+        <v>8.670693333333304</v>
       </c>
       <c r="AA155">
         <v>0.0328</v>
@@ -16236,7 +16236,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z156">
-        <v>8.472977333333336</v>
+        <v>8.470566000000012</v>
       </c>
       <c r="AA156">
         <v>0.0336</v>
@@ -16339,7 +16339,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z157">
-        <v>8.451670000000007</v>
+        <v>8.451336666666679</v>
       </c>
       <c r="AA157">
         <v>0.0324</v>
@@ -16442,7 +16442,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z158">
-        <v>8.442969333333343</v>
+        <v>8.452226000000012</v>
       </c>
       <c r="AA158">
         <v>0.0368</v>
@@ -16545,7 +16545,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z159">
-        <v>8.492798666666658</v>
+        <v>8.506077333333332</v>
       </c>
       <c r="AA159">
         <v>0.0294</v>
@@ -16648,7 +16648,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z160">
-        <v>8.571383999999986</v>
+        <v>8.579203333333313</v>
       </c>
       <c r="AA160">
         <v>0.0304</v>
@@ -16751,7 +16751,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z161">
-        <v>8.562822666666644</v>
+        <v>8.563688666666639</v>
       </c>
       <c r="AA161">
         <v>0.0444</v>
@@ -16851,7 +16851,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z162">
-        <v>8.585931333333319</v>
+        <v>8.596605999999978</v>
       </c>
       <c r="AA162">
         <v>0.0384</v>
@@ -16951,7 +16951,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z163">
-        <v>8.575599999999987</v>
+        <v>8.575775999999991</v>
       </c>
       <c r="AA163">
         <v>0.0306</v>
@@ -17054,7 +17054,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z164">
-        <v>8.606895333333311</v>
+        <v>8.594297999999979</v>
       </c>
       <c r="AA164">
         <v>0.0344</v>
@@ -17157,7 +17157,7 @@
         <v>-5</v>
       </c>
       <c r="Z165">
-        <v>8.631691999999971</v>
+        <v>8.639498666666638</v>
       </c>
       <c r="AA165">
         <v>0.0332</v>
@@ -17260,7 +17260,7 @@
         <v>-5</v>
       </c>
       <c r="Z166">
-        <v>8.67637266666663</v>
+        <v>8.676167999999967</v>
       </c>
       <c r="AA166">
         <v>0.0334</v>
@@ -17360,7 +17360,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z167">
-        <v>8.511112666666662</v>
+        <v>8.510100666666663</v>
       </c>
       <c r="AA167">
         <v>0.0312</v>
@@ -17458,7 +17458,7 @@
         <v>-5</v>
       </c>
       <c r="Z168">
-        <v>8.494708666666664</v>
+        <v>8.491271999999993</v>
       </c>
       <c r="AA168">
         <v>0.03</v>
@@ -17561,7 +17561,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z169">
-        <v>8.739240666666676</v>
+        <v>8.741427999999992</v>
       </c>
       <c r="AA169">
         <v>0.028</v>
@@ -17664,7 +17664,7 @@
         <v>-6</v>
       </c>
       <c r="Z170">
-        <v>8.612067333333336</v>
+        <v>8.590491999999999</v>
       </c>
       <c r="AA170">
         <v>0.029</v>
@@ -17767,7 +17767,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z171">
-        <v>8.750953333333358</v>
+        <v>8.768252666666694</v>
       </c>
       <c r="AA171">
         <v>0.038</v>
@@ -17867,7 +17867,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z172">
-        <v>8.39774000000001</v>
+        <v>8.386762000000013</v>
       </c>
       <c r="AA172">
         <v>0.057</v>
@@ -17967,7 +17967,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z173">
-        <v>8.423279333333344</v>
+        <v>8.417545333333344</v>
       </c>
       <c r="AA173">
         <v>0.0352</v>
@@ -18070,7 +18070,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z174">
-        <v>8.31317733333335</v>
+        <v>8.310193333333347</v>
       </c>
       <c r="AA174">
         <v>0.0292</v>
@@ -18173,7 +18173,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z175">
-        <v>8.435284666666691</v>
+        <v>8.431178666666689</v>
       </c>
       <c r="AA175">
         <v>0.038</v>
@@ -18276,7 +18276,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z176">
-        <v>8.501106</v>
+        <v>8.48963933333334</v>
       </c>
       <c r="AA176">
         <v>0.038</v>
@@ -18379,7 +18379,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z177">
-        <v>8.550484666666655</v>
+        <v>8.540957999999986</v>
       </c>
       <c r="AA177">
         <v>0.033</v>
@@ -18482,7 +18482,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z178">
-        <v>8.426467333333356</v>
+        <v>8.422711333333369</v>
       </c>
       <c r="AA178">
         <v>0.0346</v>
@@ -18585,7 +18585,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z179">
-        <v>8.461778000000013</v>
+        <v>8.467057333333351</v>
       </c>
       <c r="AA179">
         <v>0.0338</v>
@@ -18685,7 +18685,7 @@
         <v>-5</v>
       </c>
       <c r="Z180">
-        <v>8.401113333333342</v>
+        <v>8.41012133333334</v>
       </c>
       <c r="AA180">
         <v>0.0306</v>
@@ -18788,7 +18788,7 @@
         <v>-5</v>
       </c>
       <c r="Z181">
-        <v>8.46309133333334</v>
+        <v>8.466396000000007</v>
       </c>
       <c r="AA181">
         <v>0.0336</v>
@@ -18891,7 +18891,7 @@
         <v>-5</v>
       </c>
       <c r="Z182">
-        <v>8.476132666666672</v>
+        <v>8.475762666666679</v>
       </c>
       <c r="AA182">
         <v>0.0452</v>
@@ -18994,7 +18994,7 @@
         <v>-5</v>
       </c>
       <c r="Z183">
-        <v>8.545854666666656</v>
+        <v>8.550611333333327</v>
       </c>
       <c r="AA183">
         <v>0.0318</v>
@@ -19097,7 +19097,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z184">
-        <v>8.502913333333328</v>
+        <v>8.506319333333323</v>
       </c>
       <c r="AA184">
         <v>0.0316</v>
@@ -19200,7 +19200,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z185">
-        <v>8.49753733333333</v>
+        <v>8.496791333333331</v>
       </c>
       <c r="AA185">
         <v>0.0396</v>
@@ -19300,7 +19300,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z186">
-        <v>8.497466000000001</v>
+        <v>8.500670000000003</v>
       </c>
       <c r="AA186">
         <v>0.0308</v>
@@ -19403,7 +19403,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z187">
-        <v>8.308398000000034</v>
+        <v>8.31068000000003</v>
       </c>
       <c r="AA187">
         <v>0.03</v>
@@ -19506,7 +19506,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z188">
-        <v>8.39448866666668</v>
+        <v>8.40837733333335</v>
       </c>
       <c r="AA188">
         <v>0.0358</v>
@@ -19609,7 +19609,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z189">
-        <v>8.474527333333333</v>
+        <v>8.485845999999999</v>
       </c>
       <c r="AA189">
         <v>0.0556</v>
@@ -19712,7 +19712,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z190">
-        <v>8.444442666666681</v>
+        <v>8.444421333333336</v>
       </c>
       <c r="AA190">
         <v>0.0382</v>
@@ -19815,7 +19815,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z191">
-        <v>8.346173333333361</v>
+        <v>8.34449333333334</v>
       </c>
       <c r="AA191">
         <v>0.0368</v>
@@ -19918,7 +19918,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z192">
-        <v>8.356451333333354</v>
+        <v>8.350542666666678</v>
       </c>
       <c r="AA192">
         <v>0.0412</v>
@@ -20021,7 +20021,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z193">
-        <v>8.433794666666659</v>
+        <v>8.432650666666659</v>
       </c>
       <c r="AA193">
         <v>0.0318</v>
@@ -20124,7 +20124,7 @@
         <v>-5</v>
       </c>
       <c r="Z194">
-        <v>8.509437333333336</v>
+        <v>8.499474000000003</v>
       </c>
       <c r="AA194">
         <v>0.0476</v>
@@ -20224,7 +20224,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z195">
-        <v>8.488056000000006</v>
+        <v>8.497898666666671</v>
       </c>
       <c r="AA195">
         <v>0.0504</v>
@@ -20327,7 +20327,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z196">
-        <v>8.486322000000015</v>
+        <v>8.492582000000008</v>
       </c>
       <c r="AA196">
         <v>0.0332</v>
@@ -20430,7 +20430,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z197">
-        <v>8.319114666666676</v>
+        <v>8.327268000000014</v>
       </c>
       <c r="AA197">
         <v>0.0326</v>
@@ -20533,7 +20533,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z198">
-        <v>8.246498666666664</v>
+        <v>8.236651333333331</v>
       </c>
       <c r="AA198">
         <v>0.0342</v>
@@ -20636,7 +20636,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z199">
-        <v>8.196977999999987</v>
+        <v>8.20463399999999</v>
       </c>
       <c r="AA199">
         <v>0.0338</v>
@@ -20739,7 +20739,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z200">
-        <v>8.279660666666677</v>
+        <v>8.27654066666668</v>
       </c>
       <c r="AA200">
         <v>0.0434</v>
@@ -20842,7 +20842,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z201">
-        <v>8.374863333333353</v>
+        <v>8.368566000000015</v>
       </c>
       <c r="AA201">
         <v>0.0428</v>
@@ -20945,7 +20945,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z202">
-        <v>8.414892666666699</v>
+        <v>8.415194666666697</v>
       </c>
       <c r="AA202">
         <v>0.053</v>
@@ -21048,7 +21048,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z203">
-        <v>8.419163333333367</v>
+        <v>8.423554666666698</v>
       </c>
       <c r="AA203">
         <v>0.04</v>
@@ -21148,7 +21148,7 @@
         <v>-6</v>
       </c>
       <c r="Z204">
-        <v>8.436649999999997</v>
+        <v>8.440219999999989</v>
       </c>
       <c r="AA204">
         <v>0.0536</v>
@@ -21251,7 +21251,7 @@
         <v>-6.2</v>
       </c>
       <c r="Z205">
-        <v>8.363591333333362</v>
+        <v>8.356725333333356</v>
       </c>
       <c r="AA205">
         <v>0.0304</v>
@@ -21354,7 +21354,7 @@
         <v>-6.2</v>
       </c>
       <c r="Z206">
-        <v>8.384989333333362</v>
+        <v>8.385496000000028</v>
       </c>
       <c r="AA206">
         <v>0.0306</v>
@@ -21457,7 +21457,7 @@
         <v>-6.4</v>
       </c>
       <c r="Z207">
-        <v>8.497227333333337</v>
+        <v>8.488634666666664</v>
       </c>
       <c r="AA207">
         <v>0.0312</v>
@@ -21560,7 +21560,7 @@
         <v>-6.4</v>
       </c>
       <c r="Z208">
-        <v>8.498044000000009</v>
+        <v>8.495773333333339</v>
       </c>
       <c r="AA208">
         <v>0.0322</v>
@@ -21660,7 +21660,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z209">
-        <v>8.351280666666673</v>
+        <v>8.350173333333334</v>
       </c>
       <c r="AA209">
         <v>0.0484</v>
@@ -21758,7 +21758,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z210">
-        <v>8.462803999999995</v>
+        <v>8.478443999999989</v>
       </c>
       <c r="AA210">
         <v>0.0486</v>
@@ -21856,7 +21856,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z211">
-        <v>8.334428666666662</v>
+        <v>8.327760666666657</v>
       </c>
       <c r="AA211">
         <v>0.0348</v>
@@ -21959,7 +21959,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z212">
-        <v>8.329665333333372</v>
+        <v>8.329808666666699</v>
       </c>
       <c r="AA212">
         <v>0.046</v>
@@ -22062,7 +22062,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z213">
-        <v>8.355968666666689</v>
+        <v>8.35715533333336</v>
       </c>
       <c r="AA213">
         <v>0.0358</v>
@@ -22165,7 +22165,7 @@
         <v>-6</v>
       </c>
       <c r="Z214">
-        <v>8.399496666666685</v>
+        <v>8.408538666666688</v>
       </c>
       <c r="AA214">
         <v>0.0326</v>
@@ -22268,7 +22268,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z215">
-        <v>8.509969999999985</v>
+        <v>8.519026666666653</v>
       </c>
       <c r="AA215">
         <v>0.0158</v>
@@ -22371,7 +22371,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z216">
-        <v>8.417985333333339</v>
+        <v>8.41149533333334</v>
       </c>
       <c r="AA216">
         <v>0.0114</v>
@@ -22474,7 +22474,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z217">
-        <v>8.394160000000001</v>
+        <v>8.382403333333325</v>
       </c>
       <c r="AA217">
         <v>0.03</v>
@@ -22577,7 +22577,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z218">
-        <v>8.36391666666669</v>
+        <v>8.364049333333353</v>
       </c>
       <c r="AA218">
         <v>0.0026</v>
@@ -22680,7 +22680,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z219">
-        <v>8.330540666666694</v>
+        <v>8.32179866666668</v>
       </c>
       <c r="AA219">
         <v>0.0048</v>
@@ -22783,7 +22783,7 @@
         <v>-5</v>
       </c>
       <c r="Z220">
-        <v>8.49875066666667</v>
+        <v>8.495281333333336</v>
       </c>
       <c r="AA220">
         <v>0.008999999999999999</v>
@@ -22886,7 +22886,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z221">
-        <v>8.547562666666662</v>
+        <v>8.549763999999994</v>
       </c>
       <c r="AA221">
         <v>0.0094</v>
@@ -22989,7 +22989,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z222">
-        <v>8.476441333333344</v>
+        <v>8.477235333333342</v>
       </c>
       <c r="AA222">
         <v>0.0026</v>
@@ -23092,7 +23092,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z223">
-        <v>8.469238666666678</v>
+        <v>8.472766000000011</v>
       </c>
       <c r="AA223">
         <v>0.0026</v>
@@ -23195,7 +23195,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z224">
-        <v>8.469920000000005</v>
+        <v>8.472638000000009</v>
       </c>
       <c r="AA224">
         <v>0.0026</v>
@@ -23298,7 +23298,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z225">
-        <v>8.360848000000015</v>
+        <v>8.371493333333349</v>
       </c>
       <c r="AA225">
         <v>0.0026</v>
@@ -23401,7 +23401,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z226">
-        <v>8.580552666666643</v>
+        <v>8.588964666666644</v>
       </c>
       <c r="AA226">
         <v>0.0154</v>
@@ -23504,7 +23504,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z227">
-        <v>8.487316666666676</v>
+        <v>8.474702000000011</v>
       </c>
       <c r="AA227">
         <v>0.0066</v>
@@ -23601,7 +23601,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z228">
-        <v>8.478480666666671</v>
+        <v>8.475480666666673</v>
       </c>
       <c r="AA228">
         <v>0.0036</v>
@@ -23704,7 +23704,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z229">
-        <v>8.490426666666675</v>
+        <v>8.497455333333338</v>
       </c>
       <c r="AA229">
         <v>0.0048</v>
@@ -23807,7 +23807,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z230">
-        <v>8.493754666666669</v>
+        <v>8.496804000000001</v>
       </c>
       <c r="AA230">
         <v>0.0026</v>
@@ -23910,7 +23910,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z231">
-        <v>8.471484666666678</v>
+        <v>8.475132666666669</v>
       </c>
       <c r="AA231">
         <v>0.0026</v>
@@ -24013,7 +24013,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z232">
-        <v>8.481660000000002</v>
+        <v>8.480670666666668</v>
       </c>
       <c r="AA232">
         <v>0.0026</v>
@@ -24113,7 +24113,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z233">
-        <v>8.516651999999993</v>
+        <v>8.517633999999989</v>
       </c>
       <c r="AA233">
         <v>0.0196</v>
@@ -24216,7 +24216,7 @@
         <v>-5</v>
       </c>
       <c r="Z234">
-        <v>8.503615999999999</v>
+        <v>8.507319333333328</v>
       </c>
       <c r="AA234">
         <v>0.023</v>
@@ -24319,7 +24319,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z235">
-        <v>8.578450666666646</v>
+        <v>8.580731333333308</v>
       </c>
       <c r="AA235">
         <v>0.0218</v>
@@ -24422,7 +24422,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z236">
-        <v>8.588130666666645</v>
+        <v>8.592013333333309</v>
       </c>
       <c r="AA236">
         <v>0.0282</v>
@@ -24520,7 +24520,7 @@
         <v>-5</v>
       </c>
       <c r="Z237">
-        <v>8.52835266666666</v>
+        <v>8.539981333333328</v>
       </c>
       <c r="AA237">
         <v>0.0166</v>
@@ -24623,7 +24623,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z238">
-        <v>8.626604666666648</v>
+        <v>8.622321999999984</v>
       </c>
       <c r="AA238">
         <v>0.0162</v>
@@ -24726,7 +24726,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z239">
-        <v>8.665705999999973</v>
+        <v>8.665545333333293</v>
       </c>
       <c r="AA239">
         <v>0.0126</v>
@@ -24829,7 +24829,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z240">
-        <v>8.487632666666665</v>
+        <v>8.499509999999994</v>
       </c>
       <c r="AA240">
         <v>0.0102</v>
@@ -24932,7 +24932,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z241">
-        <v>8.504198666666662</v>
+        <v>8.497538666666664</v>
       </c>
       <c r="AA241">
         <v>0.0108</v>
@@ -25035,7 +25035,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z242">
-        <v>8.510137999999996</v>
+        <v>8.507990666666657</v>
       </c>
       <c r="AA242">
         <v>0.0124</v>
@@ -25138,7 +25138,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z243">
-        <v>8.54983599999998</v>
+        <v>8.545065333333319</v>
       </c>
       <c r="AA243">
         <v>0.009599999999999999</v>
@@ -25238,7 +25238,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z244">
-        <v>8.525187999999995</v>
+        <v>8.521052666666657</v>
       </c>
       <c r="AA244">
         <v>0.0292</v>
@@ -25341,7 +25341,7 @@
         <v>-5</v>
       </c>
       <c r="Z245">
-        <v>8.531759333333323</v>
+        <v>8.528935999999996</v>
       </c>
       <c r="AA245">
         <v>0.0118</v>
@@ -25444,7 +25444,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z246">
-        <v>8.402047333333375</v>
+        <v>8.403398666666709</v>
       </c>
       <c r="AA246">
         <v>0.0042</v>
@@ -25547,7 +25547,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z247">
-        <v>8.404008000000038</v>
+        <v>8.402425333333371</v>
       </c>
       <c r="AA247">
         <v>0.0062</v>
@@ -25650,7 +25650,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z248">
-        <v>8.412228666666696</v>
+        <v>8.41029133333336</v>
       </c>
       <c r="AA248">
         <v>0.0024</v>
@@ -25753,7 +25753,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z249">
-        <v>8.531841333333324</v>
+        <v>8.526842666666658</v>
       </c>
       <c r="AA249">
         <v>0.0024</v>
@@ -25850,7 +25850,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z250">
-        <v>8.565931999999989</v>
+        <v>8.568643999999992</v>
       </c>
       <c r="AA250">
         <v>0.0026</v>
@@ -25953,7 +25953,7 @@
         <v>-6</v>
       </c>
       <c r="Z251">
-        <v>8.485124000000008</v>
+        <v>8.488286666666665</v>
       </c>
       <c r="AA251">
         <v>0.0026</v>
@@ -26053,7 +26053,7 @@
         <v>-5</v>
       </c>
       <c r="Z252">
-        <v>8.457272666666679</v>
+        <v>8.458344000000013</v>
       </c>
       <c r="AA252">
         <v>0.0026</v>
@@ -26156,7 +26156,7 @@
         <v>-5</v>
       </c>
       <c r="Z253">
-        <v>8.460996666666677</v>
+        <v>8.459754666666674</v>
       </c>
       <c r="AA253">
         <v>0.006</v>
@@ -26253,7 +26253,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z254">
-        <v>8.486423333333331</v>
+        <v>8.481837333333337</v>
       </c>
       <c r="AA254">
         <v>0.0196</v>
@@ -26356,7 +26356,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z255">
-        <v>8.577380666666652</v>
+        <v>8.59836333333331</v>
       </c>
       <c r="AA255">
         <v>0.0476</v>
@@ -26459,7 +26459,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z256">
-        <v>8.541899333333328</v>
+        <v>8.537798666666655</v>
       </c>
       <c r="AA256">
         <v>0.0136</v>
@@ -26542,7 +26542,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z257">
-        <v>8.509334666666669</v>
+        <v>8.528367333333325</v>
       </c>
       <c r="AA257">
         <v>0.011</v>
@@ -26634,7 +26634,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z258">
-        <v>8.520345333333324</v>
+        <v>8.524839333333317</v>
       </c>
       <c r="AA258">
         <v>0.0282</v>
@@ -26737,7 +26737,7 @@
         <v>-6</v>
       </c>
       <c r="Z259">
-        <v>8.634641999999966</v>
+        <v>8.637608666666635</v>
       </c>
       <c r="AA259">
         <v>0.0148</v>
@@ -26840,7 +26840,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z260">
-        <v>8.517034666666657</v>
+        <v>8.518050666666657</v>
       </c>
       <c r="AA260">
         <v>0.0108</v>
@@ -26943,7 +26943,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z261">
-        <v>8.504841999999988</v>
+        <v>8.509230000000006</v>
       </c>
       <c r="AA261">
         <v>0.0026</v>
@@ -27046,7 +27046,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z262">
-        <v>8.611532666666633</v>
+        <v>8.605737333333316</v>
       </c>
       <c r="AA262">
         <v>0.0026</v>
@@ -27149,7 +27149,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z263">
-        <v>8.631339999999971</v>
+        <v>8.639864666666636</v>
       </c>
       <c r="AA263">
         <v>0.0074</v>
@@ -27252,7 +27252,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z264">
-        <v>8.46744733333334</v>
+        <v>8.469177333333342</v>
       </c>
       <c r="AA264">
         <v>0.0038</v>
@@ -27355,7 +27355,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z265">
-        <v>8.601297333333305</v>
+        <v>8.606796666666645</v>
       </c>
       <c r="AA265">
         <v>0.0024</v>
@@ -27458,7 +27458,7 @@
         <v>-6.2</v>
       </c>
       <c r="Z266">
-        <v>8.272139333333346</v>
+        <v>8.244218000000014</v>
       </c>
       <c r="AA266">
         <v>0.0068</v>
@@ -27561,7 +27561,7 @@
         <v>-6</v>
       </c>
       <c r="Z267">
-        <v>8.289221999999993</v>
+        <v>8.265830000000001</v>
       </c>
       <c r="AA267">
         <v>0.0026</v>
@@ -27664,7 +27664,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z268">
-        <v>8.153173333333328</v>
+        <v>8.141198666666654</v>
       </c>
       <c r="AA268">
         <v>0.0062</v>

</xml_diff>